<commit_message>
quasi Abgabefertig (mehrere Kniffel --)
</commit_message>
<xml_diff>
--- a/Programmentwurf/docs/Bewertung.xlsx
+++ b/Programmentwurf/docs/Bewertung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e-mai\Documents\Python_2021\Python - Programmentwurf 2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/70086f12d5d9e101/Dokumente/DHBW/Programmieren/Python/Kniffel/Programmentwurf/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271C2E1D-2742-4816-B2DB-E546AB88E664}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{271C2E1D-2742-4816-B2DB-E546AB88E664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{762E7324-BD62-4B5E-A6DB-E1210D740CFA}"/>
   <bookViews>
-    <workbookView xWindow="5415" yWindow="5415" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -426,18 +426,18 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,55 +451,73 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -509,7 +527,7 @@
       </c>
       <c r="C12">
         <f>SUM(C2:C10)</f>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="D12">
         <f>SUM(D2:D10)</f>

</xml_diff>